<commit_message>
Add additional test docx and xlsx files; use Apache Tika library to detect mime type and set it in attachment upload request in SynBioClient
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
+++ b/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E310E5D-CA6B-4D34-B697-1AC6FFFF9970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9045" yWindow="450" windowWidth="14100" windowHeight="10800"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>attachment_filename</t>
   </si>
@@ -131,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,11 +454,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +605,22 @@
         <v>33</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update logback-spring.xml config and add _logs to .gitignore
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
+++ b/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E310E5D-CA6B-4D34-B697-1AC6FFFF9970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC765C99-DB4E-422B-B931-CF4FEE078CE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12540" yWindow="1455" windowWidth="14100" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>attachment_filename</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>left_flank just notes</t>
+  </si>
+  <si>
+    <t>cyano_codA_Km</t>
+  </si>
+  <si>
+    <t>cyano new notes</t>
+  </si>
+  <si>
+    <t>cyano new description</t>
   </si>
 </sst>
 </file>
@@ -455,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,6 +630,20 @@
         <v>27</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add maven plugin config for launch4j and jsign; correctly retrieve formulae from Excel cells
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
+++ b/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC765C99-DB4E-422B-B931-CF4FEE078CE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791AD45B-C625-490C-8437-1091C0D80781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="1455" windowWidth="14100" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>attachment_filename</t>
   </si>
@@ -136,13 +144,16 @@
   </si>
   <si>
     <t>cyano new description</t>
+  </si>
+  <si>
+    <t>sl0199_flatten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +165,14 @@
       <b/>
       <sz val="24"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,16 +195,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,8 +666,23 @@
         <v>35</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="str">
+        <f>_xlfn.CONCAT(B15, " is a PCR file")</f>
+        <v>flanks_short.xlsx is a PCR file</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A15" r:id="rId1" display="https://synbiohub.org/user/jhay/Johnny190421/sl0199_flatten/1.0.0" xr:uid="{6536BB8B-E236-44D1-942E-48AE2720DD1F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Use 'CONCATENATE' formula in update_designs_tz.xlsx instead of CONCAT, which is not supported by the POI library
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
+++ b/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\src\test\resources\ed\biordm\sbol\synbio\handler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791AD45B-C625-490C-8437-1091C0D80781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5658A8-8704-4C7A-9571-B10C3E26E1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="str">
-        <f>_xlfn.CONCAT(B15, " is a PCR file")</f>
+        <f>CONCATENATE(B15, " is a PCR file")</f>
         <v>flanks_short.xlsx is a PCR file</v>
       </c>
     </row>

</xml_diff>

<commit_message>
experimentation branch for Excel formulas update
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
+++ b/src/test/resources/ed/biordm/sbol/synbio/handler/update_designs_tz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Chickens\Documents\EPCC\SynthSys\code_projects\synbio-toolkit\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5658A8-8704-4C7A-9571-B10C3E26E1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E003829-B501-4F18-A791-5FD3E7F320E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>attachment_filename</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>sl0199_flatten</t>
+  </si>
+  <si>
+    <t>some new descriptive text</t>
   </si>
 </sst>
 </file>
@@ -486,21 +489,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -514,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -528,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -542,7 +545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -553,7 +556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -564,7 +567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -578,7 +581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -589,7 +592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -600,7 +603,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -611,7 +614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -625,7 +628,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -636,7 +639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -644,7 +647,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -652,7 +655,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -666,16 +669,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
+      </c>
+      <c r="C15" t="str">
+        <f>CONCATENATE("Here is some text to append: ", E15)</f>
+        <v>Here is some text to append: some new descriptive text</v>
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE(B15, " is a PCR file")</f>
         <v>flanks_short.xlsx is a PCR file</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>